<commit_message>
Análisis Geográfico v2 y bases de datos
</commit_message>
<xml_diff>
--- a/comunas_df.xlsx
+++ b/comunas_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Comuna</t>
   </si>
@@ -22,55 +22,7 @@
     <t>geometry</t>
   </si>
   <si>
-    <t>Casos</t>
-  </si>
-  <si>
-    <t>coords</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>casos-isna</t>
   </si>
   <si>
     <t>POLYGON ((-58.5033113251 -34.5938561596, -58.5021419645 -34.5931334166, -58.5019281473 -34.5930012265, -58.5008170778 -34.592315284, -58.4994872757 -34.5914941809, -58.4982024765 -34.590700938, -58.49706634 -34.5899994752, -58.4959279222 -34.5892965223, -58.4955923211 -34.5890892809, -58.4953611476 -34.5889458168, -58.4947943786 -34.5885941919, -58.4942253128 -34.5882410866, -58.4938904862 -34.5880333473, -58.4936634924 -34.5878902304, -58.4925401173 -34.5871819611, -58.4919701332 -34.5868225065, -58.4914133555 -34.586471498, -58.4908502789 -34.5861164742, -58.4902856753 -34.5857604621, -58.4895595069 -34.5853025772, -58.4889688515 -34.5849300844, -58.4887935721 -34.5848182166, -58.4881036274 -34.5844186974, -58.4870330815 -34.5837986797, -58.4859596552 -34.5831769619, -58.485824329 -34.583098533, -58.4850954075 -34.5826749192, -58.4847468322 -34.5824723693, -58.4841208843 -34.5821085924, -58.4831341099 -34.5815350762, -58.4830135212 -34.5814649521, -58.4821455612 -34.5809595798, -58.4811291788 -34.5803677409, -58.4809936905 -34.5802888144, -58.4804835909 -34.5799935256, -58.4803102714 -34.579893237, -58.4801834079 -34.5798198288, -58.4792326245 -34.5792694455, -58.4789880538 -34.5791249658, -58.4786552624 -34.5789283818, -58.4781986574 -34.5786688521, -58.4777731362 -34.5784269942, -58.4773332265 -34.5781769667, -58.4771503154 -34.5780731807, -58.475594308 -34.57719029, -58.4750068428 -34.5768569561, -58.4749787637 -34.5768409736, -58.4748508448 -34.5767681658, -58.4746189777 -34.5766361402, -58.4738290323 -34.5761864074, -58.4737344326 -34.5761348091, -58.4736847028 -34.5761076846, -58.4735471005 -34.5760327641, -58.4728866794 -34.575655059, -58.4727424361 -34.5755718278, -58.4719583859 -34.5751195465, -58.4718058854 -34.5750325828, -58.4708650051 -34.5744961471, -58.4699255789 -34.5739604854, -58.4691338171 -34.5735090256, -58.4682875652 -34.5730265119, -58.4680812614 -34.57290884, -58.4673642696 -34.5724961753, -58.4660373929 -34.5733359032, -58.4649915374 -34.5739950401, -58.4633555464 -34.5750084122, -58.4631871043 -34.5751051166, -58.4623760599 -34.5760319079, -58.4622470601 -34.5761666972, -58.4616052429 -34.5768372891, -58.4606325863 -34.5778534851, -58.4605469511 -34.5779429558, -58.460224834 -34.5782952881, -58.4601985594 -34.5782953479, -58.4601021386 -34.5782955677, -58.4597845714 -34.5783147333, -58.4596950536 -34.5783201362, -58.4585384246 -34.5783900347, -58.4577639165 -34.5784368125, -58.4577436676 -34.5784380359, -58.4573407479 -34.5785467558, -58.4571617667 -34.5785949887, -58.4571475839 -34.5785988156, -58.4559708829 -34.5789162809, -58.4553992793 -34.5790704791, -58.4548623269 -34.5792427068, -58.4535334741 -34.5796688999, -58.4530206113 -34.5798333742, -58.4521930272 -34.5800988096, -58.4521387167 -34.5801162118, -58.4520222992 -34.5801535152, -58.4512517653 -34.5804006516, -58.4510175902 -34.5804757586, -58.4510096596 -34.5804789048, -58.4509524498 -34.5805016004, -58.4505172245 -34.5806742198, -58.4499989854 -34.5808797607, -58.4496743253 -34.5810085115, -58.4495954406 -34.5810397949, -58.4494416524 -34.5810963999, -58.4491919812 -34.5811882777, -58.4484595681 -34.5814579241, -58.448393403 -34.5814822834, -58.448325823 -34.5815071661, -58.4482895615 -34.5815205168, -58.448279634 -34.5815241719, -58.4482750418 -34.5815261464, -58.4480518327 -34.581622094, -58.4470924722 -34.5820344713, -58.4461817148 -34.5824259259, -58.4457859876 -34.5825960105, -58.4446425155 -34.5830874843, -58.444471514 -34.5831609807, -58.4444485731 -34.5831708409, -58.4444069043 -34.5831887563, -58.4443997765 -34.5831918211, -58.4444002339 -34.5831933879, -58.4447856534 -34.5845135514, -58.4445857679 -34.5846657823, -58.4434772519 -34.5854009946, -58.4424251829 -34.5860987403, -58.4413975399 -34.5867802831, -58.4410892261 -34.5869846739, -58.4401565271 -34.5876011493, -58.4393890485 -34.58810835, -58.4386143205 -34.5886204031, -58.4385455946 -34.5886617713, -58.4385357501 -34.5886677008, -58.4385342391 -34.5886686101, -58.4384977208 -34.5886905936, -58.4382498657 -34.5888568896, -58.4382224542 -34.5888752889, -58.438051411 -34.588990094, -58.4371243706 -34.5896120406, -58.4361738933 -34.5902497512, -58.4360366742 -34.5903418372, -58.4353107969 -34.5908219065, -58.4343631908 -34.591448687, -58.4341326121 -34.5916011045, -58.4335394301 -34.5919959382, -58.4334455528 -34.5920584246, -58.4334256765 -34.5920716485, -58.432358646 -34.5927817087, -58.4312194189 -34.5935397599, -58.4307421171 -34.5938573786, -58.430282227 -34.5941634129, -58.4302112522 -34.5942076891, -58.4300594741 -34.5943023724, -58.4293487865 -34.5947454372, -58.4293300106 -34.5947569129, -58.4291690483 -34.5948553217, -58.4280889075 -34.5955150464, -58.4270238275 -34.5961656099, -58.4269887519 -34.5961870107, -58.4269502241 -34.5962105181, -58.4269484087 -34.5962112883, -58.4262401641 -34.5965118706, -58.4260240564 -34.5966140638, -58.4248429581 -34.597061889, -58.4235392095 -34.5976307165, -58.4235308554 -34.5976364082, -58.4233672222 -34.5977478957, -58.4237529813 -34.5978273383, -58.4249540815 -34.5978518132, -58.4263027567 -34.5978820111, -58.4264393571 -34.5978996596, -58.4265647997 -34.5979158246, -58.4267851958 -34.5979442689, -58.4277732176 -34.5983289365, -58.4278524959 -34.5983640334, -58.4279875449 -34.5984239331, -58.4285386315 -34.5986683906, -58.4285480104 -34.5986725515, -58.4291617784 -34.5989591409, -58.4292201011 -34.5989992991, -58.429428879 -34.599126191, -58.4296465765 -34.599320696, -58.4301501679 -34.5997705667, -58.4301879688 -34.5998043809, -58.4302750634 -34.599882222, -58.4310381845 -34.6007492887, -58.4311543046 -34.6008812251, -58.4318726608 -34.6016974254, -58.4321984689 -34.6020724515, -58.4322406038 -34.6021338007, -58.4331418075 -34.6025786184, -58.4333340898 -34.6026734569, -58.4338657224 -34.6029358467, -58.4339139203 -34.6029596624, -58.4349717428 -34.6034816155, -58.4351483602 -34.6035749701, -58.4353380037 -34.6036751558, -58.4366161626 -34.6042834181, -58.4368521539 -34.6043957042, -58.4370245565 -34.604477734, -58.4370522733 -34.6044909216, -58.4370532903 -34.6044914059, -58.437057354 -34.6044934719, -58.4371745576 -34.6045530539, -58.4371890966 -34.6045604407, -58.4379749764 -34.6049597124, -58.4385110442 -34.605232041, -58.4392016361 -34.605582864, -58.439285358 -34.6056058398, -58.4401415481 -34.6058405879, -58.4403350497 -34.6058936536, -58.441465234 -34.6062035153, -58.4415997164 -34.6062391032, -58.4428240219 -34.6065715037, -58.4429800528 -34.6066123761, -58.4441672392 -34.606922926, -58.4451314561 -34.6071751199, -58.4456777355 -34.6073574581, -58.4462474253 -34.6076156443, -58.4470400255 -34.6074182057, -58.4490615868 -34.6069146271, -58.4492899509 -34.6068576786, -58.4502369641 -34.6066217842, -58.4506559557 -34.6065151316, -58.4507387493 -34.6064940829, -58.4509883575 -34.6064305501, -58.4510137653 -34.6064240829, -58.4510499036 -34.6064148844, -58.451507564 -34.6062984447, -58.452015052 -34.606167288, -58.4524282466 -34.6060604882, -58.4529588149 -34.6059231321, -58.4530692041 -34.6058943371, -58.4540018021 -34.605651793, -58.4549823494 -34.6053967787, -58.4555245782 -34.6052557496, -58.4558033574 -34.6051834394, -58.4565632913 -34.6049862895, -58.4580800805 -34.6045928209, -58.4584739255 -34.6044918448, -58.4584758017 -34.6044913635, -58.4589348008 -34.6043736871, -58.4600209326 -34.6040951836, -58.4601239918 -34.6040687763, -58.4605391247 -34.6039623717, -58.4614693812 -34.6037254045, -58.4615882813 -34.6036951225, -58.4621085137 -34.6035625862, -58.4629111734 -34.603358143, -58.4630729989 -34.603316944, -58.4643593402 -34.6029914981, -58.4649457413 -34.6028431031, -58.4652785021 -34.6027589379, -58.465796934 -34.6026303999, -58.4660826793 -34.6025596156, -58.4673339934 -34.602249562, -58.4674929192 -34.602210189, -58.4675615179 -34.6021931571, -58.4687660259 -34.6018941343, -58.46891226 -34.6018603931, -58.4692921436 -34.6021651032, -58.4701944971 -34.6028061319, -58.47019905 -34.6028086286, -58.4704340962 -34.6029375301, -58.471609637 -34.6038210728, -58.4717100636 -34.6038835345, -58.4718035037 -34.6039416282, -58.4726492421 -34.6044675682, -58.4729834864 -34.6046743792, -58.4730385977 -34.6047084598, -58.4740166366 -34.6053111422, -58.4749324276 -34.6041740394, -58.4757052188 -34.6032096982, -58.4757362997 -34.6031708905, -58.4763815971 -34.602365719, -58.4769714409 -34.6015839311, -58.4774987634 -34.6008251076, -58.476669511 -34.6003562964, -58.4765530831 -34.6002904692, -58.4763923124 -34.6001995768, -58.4777284709 -34.5999109587, -58.4777938578 -34.5998968313, -58.4785428154 -34.5997350049, -58.4788312667 -34.5996709502, -58.479747253 -34.5992763037, -58.4807802386 -34.5988312081, -58.4821273622 -34.5982507673, -58.482843671 -34.5979435456, -58.4829839825 -34.5978856335, -58.4829992791 -34.5978810877, -58.4832881109 -34.597795303, -58.4834561575 -34.5977580801, -58.4834622196 -34.5977575454, -58.484853463 -34.5976347865, -58.4851810888 -34.5976073308, -58.4861304974 -34.5975374319, -58.4864869085 -34.5975112346, -58.4866810823 -34.5974969709, -58.4871433524 -34.5974629344, -58.4873536223 -34.5974474685, -58.4877982623 -34.5974163204, -58.487824526 -34.5974144769, -58.4885444671 -34.5973639801, -58.4895267456 -34.5972965817, -58.4901861671 -34.5972500953, -58.4912174976 -34.5971809127, -58.4924899238 -34.5970955701, -58.4928202155 -34.5970734172, -58.4929088408 -34.5970674728, -58.493417691 -34.597033401, -58.4947157466 -34.5969477115, -58.4967848635 -34.5968111602, -58.4971282396 -34.5967885277, -58.4971750925 -34.5968173886, -58.4971750925 -34.5968173887, -58.4983848399 -34.5963676569, -58.4995508073 -34.5959341956, -58.4996339138 -34.595903324, -58.4997866781 -34.5958465137, -58.5001263358 -34.5957202088, -58.5007096946 -34.5955034008, -58.5017928731 -34.5951008597, -58.5027574306 -34.5947423636, -58.5028766373 -34.5946980266, -58.5031804411 -34.5945821871, -58.5035437666 -34.59445012, -58.5030835155 -34.5943822421, -58.5034718173 -34.5939535747, -58.5033113251 -34.5938561596))</t>
@@ -116,51 +68,6 @@
   </si>
   <si>
     <t>POLYGON ((-58.4156625431 -34.597859783, -58.4156907176 -34.5978593657, -58.4160004849 -34.5978547719, -58.4155178134 -34.596712993, -58.4150463809 -34.5955979775, -58.4146259891 -34.5946036186, -58.414393642 -34.5940540689, -58.4135230115 -34.59307319, -58.4128778538 -34.5923197295, -58.4124629027 -34.5918351035, -58.412390824 -34.591750915, -58.4123269988 -34.5916763789, -58.4111888072 -34.590346837, -58.4100810283 -34.5890571582, -58.4094978052 -34.5882271536, -58.4091930795 -34.5877933507, -58.4090286823 -34.5875593157, -58.4083166756 -34.5865459317, -58.408136061 -34.5862888689, -58.4080382248 -34.5861491715, -58.4076257009 -34.585560512, -58.4070917855 -34.5847984776, -58.4063982017 -34.5838085422, -58.4061723613 -34.5834592684, -58.4053598508 -34.5834529741, -58.404026643 -34.5834426211, -58.4020439041 -34.5834272152, -58.4019430855 -34.5834263898, -58.4013483666 -34.5837912858, -58.4013459055 -34.5837927963, -58.4012153872 -34.583881467, -58.4011266148 -34.5839418471, -58.4005436963 -34.5844718546, -58.3999389713 -34.583641864, -58.3992749714 -34.5827304273, -58.3993615811 -34.5827150486, -58.398109295 -34.580702127, -58.3979600224 -34.5804922499, -58.3969241471 -34.5790359314, -58.3967525965 -34.5787947724, -58.3965596897 -34.5785067263, -58.3966420596 -34.5784523714, -58.3968117342 -34.5783404043, -58.3978171969 -34.5776768972, -58.3978938055 -34.5776263425, -58.3985818485 -34.5771716612, -58.3986099958 -34.5771565921, -58.3990462283 -34.5769230519, -58.3998743537 -34.5765218696, -58.3999405489 -34.5764898004, -58.400508138 -34.5761559185, -58.4006572764 -34.5760576889, -58.4011445521 -34.5757367467, -58.4012364976 -34.5756607876, -58.4016520218 -34.5753175071, -58.4021347496 -34.5747374757, -58.4024091208 -34.5744077947, -58.4026464001 -34.5741403731, -58.4025066839 -34.5740021928, -58.4024086058 -34.573902905, -58.402027689 -34.5735172865, -58.4017451747 -34.5731321603, -58.400661986 -34.5718642587, -58.4005417429 -34.5717432793, -58.4004483878 -34.5716493523, -58.4003018632 -34.5715019288, -58.3999178808 -34.5710496012, -58.3998854124 -34.5710113532, -58.3997157524 -34.5708069483, -58.3996356616 -34.5705617259, -58.3996296065 -34.5704033773, -58.399651373 -34.570199071, -58.3996978226 -34.5700177635, -58.3998060509 -34.569798178, -58.4001084367 -34.5693744414, -58.400126406 -34.5693492606, -58.4001266602 -34.5693489037, -58.3993450363 -34.5698665506, -58.3993397363 -34.5698700608, -58.3992705896 -34.5699049199, -58.3989963886 -34.5700431511, -58.3987972863 -34.5701435223, -58.3986997632 -34.5701991131, -58.3983655153 -34.5703896448, -58.3952057971 -34.5721906912, -58.3948202721 -34.5723094261, -58.394323495 -34.5722904861, -58.3943190478 -34.5722901726, -58.393532276 -34.572234678, -58.3933109382 -34.5722190646, -58.393208312 -34.5722118253, -58.3928393283 -34.5722329087, -58.3929840359 -34.5719760718, -58.3929211318 -34.57201307, -58.3915322351 -34.5728299517, -58.3904362616 -34.5734745282, -58.3894993552 -34.5740255372, -58.3885733886 -34.5745291601, -58.3861571538 -34.5758432623, -58.3853097731 -34.5763041008, -58.3834375408 -34.5761695728, -58.3830696747 -34.5758274635, -58.3828793968 -34.575650507, -58.3828515133 -34.5756198008, -58.3828301284 -34.5755857148, -58.3828158244 -34.5755491807, -58.3828089915 -34.5755111965, -58.3828098184 -34.5754728008, -58.3828182811 -34.575435042, -58.3828341476 -34.5753989513, -58.3828569865 -34.5753655172, -58.3870950357 -34.5729650774, -58.391260751 -34.5706053294, -58.3912377932 -34.5704774755, -58.3912506727 -34.5704016623, -58.3911689739 -34.5702706143, -58.3910955592 -34.5701528549, -58.3910564731 -34.5700901598, -58.3910447764 -34.5700713974, -58.3909605939 -34.5700161045, -58.3908813588 -34.5699560171, -58.3908751159 -34.5699505614, -58.3908074687 -34.5698914372, -58.3907392958 -34.5698226887, -58.3906771832 -34.569750118, -58.3906214423 -34.5696740895, -58.3905723538 -34.5695949846, -58.3905301626 -34.5695132021, -58.390495083 -34.569429152, -58.3904902626 -34.5694233051, -58.3904621289 -34.5694139819, -58.3904146901 -34.5693946123, -58.3903697861 -34.5693714735, -58.3903420045 -34.5693544125, -58.3903156104 -34.5693359073, -58.3903028885 -34.5693422937, -58.3902273423 -34.5693802169, -58.3842808791 -34.5688937058, -58.3842071279 -34.5688766517, -58.3841356815 -34.5688538487, -58.3840671958 -34.5688255055, -58.3840022939 -34.5687918821, -58.3839415715 -34.5687532853, -58.3838855819 -34.568710068, -58.383834838 -34.5686626245, -58.3838023122 -34.5686340348, -58.3837409977 -34.5685718251, -58.3836851766 -34.5685061726, -58.3836539277 -34.568493012, -58.3835505605 -34.568457016, -58.3834443149 -34.5684273057, -58.3833357464 -34.5684040355, -58.3832254271 -34.5683873284, -58.3831139355 -34.5683772722, -58.3823527223 -34.5684053945, -58.3823110417 -34.5684044855, -58.3822699357 -34.5683987045, -58.3814630622 -34.5684220495, -58.3811546437 -34.5684833082, -58.3811162159 -34.5684936338, -58.381080208 -34.5685087982, -58.3810475063 -34.5685284288, -58.3810189123 -34.5685520438, -58.3809951284 -34.5685790632, -58.3809767382 -34.5686088248, -58.3809641936 -34.568640596, -58.3808296655 -34.5691055977, -58.3807428848 -34.5693917499, -58.3807555972 -34.5696600796, -58.3807295345 -34.5697745468, -58.3807076354 -34.5700535867, -58.3807065468 -34.5701123414, -58.3803526955 -34.5700976981, -58.3803944866 -34.5686523657, -58.3803951586 -34.5686041062, -58.3803874795 -34.568556264, -58.3803716041 -34.5685098224, -58.3803523102 -34.5684667238, -58.3803269748 -34.5684258198, -58.380295957 -34.5683876892, -58.3802596942 -34.5683528689, -58.3802186972 -34.5683218503, -58.3801735431 -34.5682950703, -58.3801248711 -34.5682729077, -58.3801163519 -34.5682702598, -58.3801074164 -34.5682688349, -58.3800983183 -34.5682686737, -58.380089317 -34.5682697791, -58.3800806676 -34.5682721206, -58.3800726186 -34.5682756317, -58.3800653968 -34.5682802116, -58.3800592081 -34.5682857315, -58.3800542305 -34.5682920328, -58.3800506035 -34.5682989363, -58.380048431 -34.5683062465, -58.3800360929 -34.5683393285, -58.3800296274 -34.5683735331, -58.3800296768 -34.5684139135, -58.3800378944 -34.5684537171, -58.3800452266 -34.5684686671, -58.3800552811 -34.5684824904, -58.380067814 -34.5684948505, -58.3800825194 -34.5685054471, -58.380099039 -34.5685140211, -58.380116971 -34.5685203632, -58.3801358785 -34.5685243198, -58.3801552995 -34.5685257942, -58.3801909885 -34.5686075093, -58.3802199978 -34.5686910137, -58.3802421982 -34.5687759343, -58.3802574908 -34.5688618931, -58.3802658073 -34.5689485043, -58.3802671099 -34.5690353822, -58.3802613924 -34.5691221372, -58.3802289664 -34.5698400252, -58.3800587799 -34.5699114633, -58.3800436835 -34.5699191046, -58.3800302417 -34.5699286292, -58.3800187947 -34.5699397958, -58.3800096326 -34.5699523215, -58.3800029858 -34.569965891, -58.3799990224 -34.5699801591, -58.3799978441 -34.5699947672, -58.3799994784 -34.5700093456, -58.3800038856 -34.5700235247, -58.3800249703 -34.5703670625, -58.3798344493 -34.5703520441, -58.3795266841 -34.5703277805, -58.3795249428 -34.5703276496, -58.3795234282 -34.5703275358, -58.3795201722 -34.5703272893, -58.3795182805 -34.5703271483, -58.3795169162 -34.5703270464, -58.3795136591 -34.5703268035, -58.3795104021 -34.5703265642, -58.3795081126 -34.5703263905, -58.3795071526 -34.5703263186, -58.3795038955 -34.5703260739, -58.3795038607 -34.5703260712, -58.3795006396 -34.570325831, -58.3794987631 -34.57032569, -58.3794973847 -34.5703255926, -58.3794946278 -34.5703253834, -58.3794941298 -34.5703253461, -58.3794908705 -34.5703251032, -58.3794887151 -34.5703249431, -58.3794876135 -34.5703248594, -58.3794843586 -34.5703246147, -58.3794811037 -34.57032437, -58.3794792937 -34.5703242353, -58.3794778466 -34.5703241261, -58.3794745896 -34.5703238823, -58.3794745547 -34.5703238796, -58.3794741275 -34.5703238478, -58.3794713336 -34.5703236412, -58.3794698135 -34.5703235266, -58.3794680776 -34.5703233965, -58.3794648238 -34.5703231527, -58.3794615656 -34.570322908, -58.3794605424 -34.5703228307, -58.3794583064 -34.5703226633, -58.3794550526 -34.5703224231, -58.3794517977 -34.5703221766, -58.3794506198 -34.5703220892, -58.3794485406 -34.5703219337, -58.3794452836 -34.5703216935, -58.3794452509 -34.5703216907, -58.3794443061 -34.5703216189, -58.3794441972 -34.5703216107, -58.379442033 -34.5703214488, -58.3794408518 -34.5703213614, -58.3794387771 -34.5703212086, -58.3794355222 -34.5703209648, -58.379432264 -34.57032072, -58.3794311155 -34.5703206336, -58.379429008 -34.5703204762, -58.379425751 -34.5703202315, -58.379424172 -34.5703201133, -58.3794224972 -34.5703199904, -58.3794214413 -34.5703199122, -58.3794192401 -34.5703197475, -58.3794159819 -34.5703195055, -58.379415946 -34.5703195028, -58.3794147092 -34.5703194118, -58.3794127249 -34.5703192581, -58.3794094711 -34.5703190152, -58.3794062184 -34.570318775, -58.3794029569 -34.5703185276, -58.3793997021 -34.5703182874, -58.3793972764 -34.5703181063, -58.379396445 -34.5703180436, -58.3793946241 -34.5703179071, -58.3793931912 -34.5703177979, -58.3793899657 -34.5703175578, -58.3793899341 -34.5703175541, -58.3793879193 -34.5703174031, -58.3793866771 -34.5703173094, -58.3793834189 -34.5703170647, -58.3793801706 -34.5703168209, -58.379378451 -34.5703166917, -58.3793769146 -34.5703165771, -58.3793744105 -34.5703163888, -58.3793741947 -34.5703163724, -58.3793736946 -34.5703163342, -58.3793736586 -34.5703163315, -58.3793704015 -34.570316094, -58.3793686253 -34.5703159602, -58.3793671455 -34.5703158493, -58.3793638896 -34.5703156046, -58.3793606325 -34.5703153616, -58.379359047 -34.5703152425, -58.3793573765 -34.5703151169, -58.3793541184 -34.5703148731, -58.3793536128 -34.5703148349, -58.3793508635 -34.5703146257, -58.3793494883 -34.5703145256, -58.3793476086 -34.5703143846, -58.3793443908 -34.5703141435, -58.3793443515 -34.5703141408, -58.3793410955 -34.5703138961, -58.3793400985 -34.5703138197, -58.3793378396 -34.5703136441, -58.3793345847 -34.5703134039, -58.3793327671 -34.5703132657, -58.3793313331 -34.5703131583, -58.379328076 -34.5703129163, -58.3793258596 -34.5703127507, -58.37932482 -34.5703126707, -58.379321563 -34.570312426, -58.379318307 -34.5703121822, -58.3793163172 -34.570312033, -58.379315051 -34.5703119384, -58.379311795 -34.5703116891, -58.379311758 -34.5703116864, -58.379311272 -34.57031165, -58.3793085391 -34.5703114453, -58.379307226 -34.5703113453, -58.379305282 -34.570311197, -58.3793020315 -34.5703109478, -58.3793003065 -34.5703108168, -58.3792988115 -34.5703107013, -58.3792987755 -34.5703106986, -58.3792955184 -34.5703104539, -58.3792939079 -34.5703103275, -58.3792922625 -34.5703101992, -58.3792890076 -34.57030995, -58.3792857582 -34.570309699, -58.3792825 -34.570309448, -58.3792809156 -34.570309327, -58.3792792429 -34.5703091996, -58.3792759859 -34.5703089513, -58.3792727321 -34.5703086967, -58.379269475 -34.5703084493, -58.3792678601 -34.5703083256, -58.3792662234 -34.5703082001, -58.3792629653 -34.5703079517, -58.3792616097 -34.570307848, -58.3792597104 -34.5703077016, -58.3792564555 -34.5703074551, -58.3792544396 -34.5703073005, -58.3792531995 -34.5703072059, -58.3792499403 -34.570306953, -58.3792493551 -34.5703069085, -58.3792466843 -34.5703067083, -58.3792455456 -34.5703066228, -58.3792434305 -34.5703064627, -58.3792401822 -34.570306218, -58.3792369186 -34.5703059661, -58.3792368761 -34.5703059615, -58.379233667 -34.5703057168, -58.3792323539 -34.5703056168, -58.3792304099 -34.5703054685, -58.3792271561 -34.5703052211, -58.379223898 -34.5703049719, -58.379220642 -34.5703047227, -58.3792189966 -34.5703045971, -58.379217386 -34.5703044752, -58.37921413 -34.570304226, -58.3792108784 -34.5703039822, -58.3792097582 -34.5703038958, -58.3792095741 -34.5703038831, -58.3792076595 -34.5703037357, -58.3792076225 -34.570303733, -58.3792043665 -34.5703034892, -58.3792029793 -34.5703033882, -58.3792029368 -34.5703033854, -58.3792011094 -34.570303249, -58.3791998421 -34.5703031579, -58.3791978534 -34.5703030115, -58.3791950529 -34.5703028067, -58.3791946007 -34.570302773, -58.3791913404 -34.5703025319, -58.3791891893 -34.5703023781, -58.3791880833 -34.5703022998, -58.3791868628 -34.5703022125, -58.3791848251 -34.5703020614, -58.3791831001 -34.5703019449, -58.379181567 -34.5703018338, -58.3791797101 -34.5703017037, -58.3791787065 -34.5703016327, -58.379178311 -34.5703016072, -58.3791772376 -34.5703015298, -58.3791750495 -34.5703013714, -58.3791717936 -34.5703011276, -58.3791685376 -34.5703008793, -58.3791652805 -34.570300622, -58.3791637768 -34.5703005047, -58.3791620169 -34.5703003673, -58.3791587632 -34.5703001064, -58.3791562743 -34.5702999109, -58.3791555094 -34.570299849, -58.3791523765 -34.5702995972, -58.3791522861 -34.5702995899, -58.3791522458 -34.5702995872, -58.3791489866 -34.5702993281, -58.3791457328 -34.570299077, -58.3791441146 -34.5702989542, -58.3791424713 -34.5702988287, -58.3791394246 -34.570298604, -58.3791392524 -34.5702985912, -58.3791392154 -34.5702985876, -58.3791359539 -34.5702983582, -58.3791326914 -34.5702981342, -58.3791294365 -34.5702979264, -58.3791261739 -34.5702977304, -58.3791229124 -34.5702975524, -58.3791196509 -34.5702973888, -58.3791184457 -34.5702973348, -58.3791163948 -34.570297245, -58.3791140748 -34.570297156, -58.3791131333 -34.5702971202, -58.3791130919 -34.5702971193, -58.3791098695 -34.570297017, -58.3791066058 -34.5702969345, -58.3791033431 -34.57029688, -58.3791006623 -34.5702968493, -58.3791000738 -34.5702968426, -58.3790968089 -34.5702968224, -58.3790951437 -34.5702968257, -58.3790935418 -34.5702968291, -58.3790915028 -34.5702968422, -58.3790902681 -34.5702968485, -58.379087002 -34.5702968914, -58.3790849325 -34.5702969287, -58.3790837294 -34.5702969504, -58.3790804568 -34.5702970221, -58.3790771841 -34.5702971181, -58.3790739125 -34.5702972259, -58.3790726472 -34.5702972737, -58.3790721972 -34.5702972896, -58.3790717885 -34.5702973046, -58.3790706409 -34.5702973525, -58.379068761 -34.5702974306, -58.3790687218 -34.5702974323, -58.3790673726 -34.57029749, -58.3790640988 -34.5702976455, -58.3790608347 -34.5702978155, -58.3790575707 -34.570297998, -58.3790575336 -34.5702979998, -58.3790543034 -34.570298195, -58.3790529302 -34.5702982833, -58.379051047 -34.5702984037, -58.3790478232 -34.5702986178, -58.3790477851 -34.5702986205, -58.379044533 -34.5702988572, -58.3790432611 -34.5702989528, -58.3790412874 -34.5702991019, -58.3790396101 -34.5702992459, -58.3790380353 -34.570299381, -58.379034794 -34.5702996952, -58.3790315581 -34.5703000463, -58.3790283233 -34.5703004209, -58.3790271855 -34.5703005625, -58.3790256967 -34.5703007463, -58.3790250874 -34.5703008189, -58.3790233588 -34.5703010449, -58.379021858 -34.5703012422, -58.379018633 -34.5703016808, -58.3790154024 -34.570302132, -58.3790121784 -34.5703025868, -58.3790089534 -34.5703030462, -58.3790075703 -34.5703032435, -58.3790075321 -34.5703032489, -58.3790057272 -34.5703035055, -58.3790024978 -34.5703039603, -58.3789992727 -34.5703044088, -58.3789978743 -34.570304599, -58.3789960422 -34.5703048474, -58.3789928106 -34.5703052617, -58.3789918613 -34.5703053809, -58.3789918297 -34.5703053845, -58.3789895769 -34.5703056615, -58.3789863388 -34.5703060388, -58.3789830986 -34.5703063971, -58.3789798529 -34.5703067402, -58.378978156 -34.5703069193, -58.3789766127 -34.5703070814, -58.3789733627 -34.5703074154, -58.3789701192 -34.5703077476, -58.3789668703 -34.5703080807, -58.3789650567 -34.5703082715, -58.378963629 -34.5703084219, -58.3789603877 -34.5703087767, -58.3789578275 -34.570309067, -58.3789571474 -34.5703091432, -58.3789571038 -34.5703091494, -58.3789568564 -34.570309179, -58.3789550036 -34.5703094022, -58.3789539115 -34.570309534, -58.3789526548 -34.5703096963, -58.3789506865 -34.57030995, -58.3789474614 -34.5703103877, -58.3789462113 -34.5703105717, -58.3789442418 -34.5703108606, -58.3789415278 -34.5703112752, -58.3789410254 -34.5703113506, -58.3789404761 -34.5703114385, -58.3789378188 -34.5703118559, -58.3789362035 -34.5703121135, -58.3789346111 -34.5703123684, -58.378931399 -34.570312889, -58.3789282415 -34.5703134169, -58.3789281968 -34.5703134241, -58.3789249945 -34.5703139628, -58.3789217889 -34.5703145132, -58.378918591 -34.5703150699, -58.3789165332 -34.5703154335, -58.3789153909 -34.5703156374, -58.3789122365 -34.5703162013, -58.3789121929 -34.5703162094, -58.3789090004 -34.5703167887, -58.3789058515 -34.5703173643, -58.3789058079 -34.5703173724, -58.3789026143 -34.5703179598, -58.3789005314 -34.5703183496, -58.3788994262 -34.5703185561, -58.3788962325 -34.5703191525, -58.3788930455 -34.5703197579, -58.3788914574 -34.5703200615, -58.3788898606 -34.5703203633, -58.3788866811 -34.5703209705, -58.3788834907 -34.5703215885, -58.3788821261 -34.5703218508, -58.3788803113 -34.5703221993, -58.378877122 -34.5703228119, -58.3788739393 -34.5703234308, -58.3788723708 -34.570323738, -58.3788707576 -34.5703240524, -58.3788675716 -34.5703246758, -58.3788674299 -34.5703247046, -58.3788643921 -34.5703253028, -58.3788612148 -34.5703259389, -58.3788595569 -34.5703262758, -58.3788580375 -34.5703265839, -58.3788548602 -34.5703272344, -58.3788517221 -34.570327884, -58.3788516872 -34.5703278912, -58.3788485164 -34.5703285588, -58.3788465958 -34.5703289721, -58.3788453532 -34.5703292372, -58.3788435427 -34.5703296335, -58.3788421922 -34.5703299282, -58.3788390323 -34.5703306301, -58.3788358821 -34.5703313455, -58.3788327363 -34.5703320735, -58.378829596 -34.5703328204, -58.378826461 -34.5703335791, -58.3788233294 -34.5703343549, -58.378820202 -34.5703351424, -58.3788201573 -34.5703351541, -58.3788170834 -34.5703359417, -58.3788139593 -34.570336749, -58.3788108461 -34.5703375744, -58.3788108069 -34.5703375852, -58.3788077329 -34.570338407, -58.378804624 -34.5703392567, -58.3788015272 -34.5703401155, -58.3787984292 -34.5703409914, -58.3787983954 -34.5703410013, -58.3787953366 -34.5703418799, -58.3787922495 -34.5703427783, -58.3787891678 -34.5703436876, -58.3787891329 -34.5703436983, -58.3787860937 -34.5703446121, -58.3787849993 -34.5703449503, -58.3787830305 -34.5703455538, -58.3787808808 -34.5703462203, -58.3787799695 -34.5703465019, -58.3787769128 -34.5703474697, -58.3787738703 -34.5703484439, -58.3787708365 -34.5703494415, -58.3787678092 -34.5703504554, -58.3787647895 -34.5703514881, -58.3787617785 -34.5703525372, -58.3787587751 -34.570353606, -58.3787557772 -34.5703546821, -58.3787527825 -34.5703557708, -58.3787497955 -34.5703568748, -58.3787468149 -34.5703579869, -58.3787467735 -34.5703580022, -58.3787438322 -34.5703591009, -58.3787425196 -34.5703595976, -58.3787408582 -34.5703602229, -58.378737882 -34.5703613468, -58.3787349069 -34.570362477, -58.3787329565 -34.5703632202, -58.3787319372 -34.5703636044, -58.3787309408 -34.5703639833, -58.3787308972 -34.5703639995, -58.378728961 -34.5703647301, -58.378725987 -34.5703658531, -58.3787230097 -34.5703669751, -58.3787200412 -34.57036809, -58.37871929 -34.5703683662, -58.3787170476 -34.5703691985, -58.3787170094 -34.5703692129, -58.3787151092 -34.5703699201, -58.3787150133 -34.5703699561, -58.3787149719 -34.5703699714, -58.378714067 -34.5703703061, -58.378711081 -34.5703714101, -58.3787080972 -34.5703725115, -58.3787051047 -34.5703736155, -58.3787033921 -34.5703742462, -58.3787021177 -34.5703747141, -58.3786991295 -34.5703758181, -58.3786961457 -34.5703769185, -58.3786931597 -34.5703780225, -58.3786920194 -34.5703784454, -58.3786901737 -34.5703791293, -58.3786880773 -34.5703799112, -58.3786871932 -34.5703802414, -58.3786842116 -34.5703813571, -58.3786812288 -34.5703824756, -58.3786782614 -34.5703836022, -58.3786752895 -34.5703847314, -58.3786723253 -34.5703858733, -58.3786710007 -34.5703863898, -58.3786693665 -34.5703870215, -58.3786664121 -34.570388177, -58.3786634991 -34.5703893324, -58.3786634674 -34.570389345, -58.378660525 -34.5703905203, -58.3786575923 -34.5703917109, -58.3786564945 -34.5703921599, -58.3786556692 -34.5703924956, -58.378655571 -34.570392537, -58.3786554653 -34.5703925802, -58.378654664 -34.5703929096, -58.3786537722 -34.5703932813, -58.3786534408 -34.5703934208, -58.3786517422 -34.5703941272, -58.3786488356 -34.5703953575, -58.378645941 -34.5703966067, -58.3786430486 -34.5703978713, -58.378640203 -34.5703991394, -58.3786401692 -34.5703991547, -58.3786372997 -34.5704004508, -58.378634441 -34.5704017596, -58.3786315856 -34.5704030845, -58.3786287399 -34.5704044203, -58.3786259019 -34.5704057651, -58.3786230704 -34.570407119, -58.3786202422 -34.5704084836, -58.3786174281 -34.5704098564, -58.3786169985 -34.5704100661, -58.3786146097 -34.5704112319, -58.3786145748 -34.5704112508, -58.3786137865 -34.5704116387, -58.3786125773 -34.5704122365, -58.3786118 -34.5704126181, -58.3786089946 -34.5704140062, -58.3786061892 -34.5704154007, -58.3786033904 -34.5704167924, -58.3786005992 -34.5704182003, -58.3785988219 -34.5704191032, -58.3785978156 -34.5704196155, -58.3785950418 -34.5704210369, -58.3785922668 -34.5704224755, -58.3785894996 -34.5704239195, -58.3785867802 -34.5704253483, -58.378586741 -34.570425369, -58.37858399 -34.5704268256, -58.378581238 -34.5704282895, -58.3785811976 -34.5704283111, -58.3785784947 -34.570429756, -58.3785757437 -34.5704312208, -58.3785757154 -34.570431237, -58.3785743208 -34.5704319852, -58.3785730015 -34.5704326937, -58.3785702527 -34.5704341675, -58.3785675126 -34.5704356394, -58.3785647725 -34.5704371132, -58.3785647355 -34.570437133, -58.3785620303 -34.5704385852, -58.3785592826 -34.5704400536, -58.3785574137 -34.5704410538, -58.378556536 -34.5704415228, -58.3785512063 -34.5704443479, -58.3767766935 -34.5714438657, -58.3761150489 -34.5718165322, -58.3758766442 -34.5719506442, -58.3758464803 -34.5719691926, -58.3758464443 -34.5719692178, -58.3758414879 -34.5719724469, -58.3758179903 -34.5719877583, -58.3757967041 -34.5720018157, -58.3741438695 -34.5730697111, -58.3741438401 -34.5730697282, -58.3741074986 -34.5730901917, -58.3740952724 -34.5730970762, -58.3740461822 -34.5731248141, -58.3740148818 -34.5731424931, -58.3739721769 -34.5731660015, -58.3739721463 -34.5731660186, -58.373949939 -34.5731786561, -58.3716313234 -34.5744981659, -58.3716312797 -34.5744981911, -58.3716201563 -34.5745048878, -58.371569334 -34.5745354819, -58.3715692903 -34.5745355071, -58.3715373503 -34.574554045, -58.3715170745 -34.5745658027, -58.3714977385 -34.5745761414, -58.3714949927 -34.5745776087, -58.3714935729 -34.5745783675, -58.3714735466 -34.5745890663, -58.3714459374 -34.5746047668, -58.3714238613 -34.5746173219, -58.3713772531 -34.5746430756, -58.3713284205 -34.5746717736, -58.3713283921 -34.5746717907, -58.3712876698 -34.5746957333, -58.3712876283 -34.5746957585, -58.3712641997 -34.5747102984, -58.371248247 -34.5747201951, -58.3712169695 -34.5747396492, -58.3712169455 -34.5747396664, -58.3711943741 -34.5747557015, -58.3711783826 -34.5747670649, -58.3711783499 -34.574767091, -58.3711618095 -34.5747801423, -58.3711600261 -34.5747815499, -58.3711593498 -34.5747820831, -58.3711470547 -34.5747917825, -58.3711366963 -34.5748003673, -58.3711224186 -34.5748122007, -58.3711223902 -34.5748122304, -58.3711008241 -34.5748346999, -58.3711007543 -34.5748347701, -58.3711693139 -34.5748976181, -58.3711899976 -34.5748788096, -58.3711900292 -34.5748787772, -58.3712110429 -34.574860161, -58.3712110735 -34.5748601367, -58.3712434487 -34.5748354793, -58.3712434792 -34.5748354514, -58.3712544474 -34.5748272655, -58.3712683781 -34.5748168633, -58.3712827363 -34.5748070934, -58.3712963235 -34.5747978448, -58.3713312314 -34.5747761208, -58.3713312729 -34.5747760965, -58.3713720099 -34.574751696, -58.3714130497 -34.5747275048, -58.3714407954 -34.574712649, -58.3714666219 -34.5746988221, -58.3714666699 -34.5746987924, -58.3715395084 -34.5746547129, -58.3715989788 -34.5746228506, -58.3716006265 -34.5746219675, -58.3739242576 -34.5732918546, -58.3739258898 -34.5732909202, -58.3741924445 -34.5731383311, -58.3742143367 -34.5731257988, -58.3745843164 -34.5728887976, -58.3755298517 -34.5722831021, -58.3758346144 -34.5720878731, -58.3758543444 -34.5720717314, -58.3758694915 -34.5720621734, -58.3758808818 -34.5720549843, -58.375909383 -34.5720372677, -58.3759132738 -34.5720348474, -58.3759294133 -34.5720246968, -58.3759481884 -34.572012894, -58.3759791763 -34.5719952657, -58.3760123973 -34.5719753628, -58.3760382305 -34.5719619956, -58.3760534117 -34.5719541367, -58.3760815978 -34.5719385509, -58.376105305 -34.5719270409, -58.3761118792 -34.5719253941, -58.3761156007 -34.5719244611, -58.3761158362 -34.5719244017, -58.3774743945 -34.5711538662, -58.3785466177 -34.5705457106, -58.3785466536 -34.5705456899, -58.3785765907 -34.5705283577, -58.3785964928 -34.5705168293, -58.3786095561 -34.5705100252, -58.378610568 -34.5705094976, -58.378613767 -34.5705078294, -58.3786364396 -34.570496019, -58.3786794169 -34.5704752729, -58.3786794442 -34.5704752594, -58.378709782 -34.5704613746, -58.378709818 -34.5704613593, -58.3787434018 -34.5704457594, -58.3787434509 -34.570445736, -58.3787434956 -34.5704457153, -58.378775501 -34.5704348271, -58.3787997708 -34.5704265703, -58.3788377857 -34.5704162568, -58.3788693657 -34.5704078878, -58.3789126079 -34.5703989589, -58.3789142931 -34.5703986103, -58.3789513782 -34.5703917172, -58.3789889951 -34.5703859755, -58.3790115305 -34.5703837166, -58.3790123523 -34.5703836342, -58.3790529916 -34.5703795596, -58.379065413 -34.5703792761, -58.3790673932 -34.5703792296, -58.3790697319 -34.5703791763, -58.3790924257 -34.5703786608, -58.379139326 -34.5703785821, -58.3791542496 -34.570379372, -58.3791678655 -34.570380089, -58.3791850176 -34.5703809941, -58.3791850579 -34.570380995, -58.3792236044 -34.5703838582, -58.3792459942 -34.5703855169, -58.379964056 -34.5704424984, -58.3803558677 -34.5704735884, -58.3803253705 -34.5708095308, -58.380501704 -34.5710380664, -58.3802630426 -34.5711755681, -58.3789049335 -34.5719580106, -58.3784188716 -34.5722380368, -58.3783036496 -34.5723044163, -58.3782979087 -34.5723129725, -58.3782978814 -34.5723130139, -58.3782978061 -34.5723131194, -58.3782935566 -34.5723188911, -58.378292618 -34.5723223727, -58.3782917123 -34.57232573, -58.3782891292 -34.5723313839, -58.3782864195 -34.5723373108, -58.3782855237 -34.5723426504, -58.3782847716 -34.5723471292, -58.3782487684 -34.5726561022, -58.378246506 -34.5726755132, -58.3782465362 -34.5726758261, -58.3782472298 -34.5726828795, -58.3782480388 -34.5726911129, -58.3782496656 -34.5726967959, -58.3782515291 -34.5727033038, -58.3782515954 -34.57270354, -58.3782517432 -34.57270388, -58.3782560465 -34.5727139269, -58.3782560617 -34.5727139539, -58.3782609506 -34.5727224805, -58.3782610866 -34.5727227186, -58.378261337 -34.5727230298, -58.3782613827 -34.5727230866, -58.378267812 -34.5727310832, -58.3782775295 -34.5727410464, -58.3782777744 -34.5727412972, -58.3782778115 -34.5727413306, -58.3782789136 -34.5727420868, -58.3782816449 -34.5727439646, -58.3782870792 -34.572747685, -58.3782963267 -34.5727536662, -58.3782979973 -34.5727547464, -58.3782982086 -34.5727548727, -58.3782982598 -34.5727549025, -58.3783086545 -34.5727611234, -58.378308697 -34.5727611378, -58.3783216395 -34.572765407, -58.3783218628 -34.5727654802, -58.3783219021 -34.5727654892, -58.3783229143 -34.5727656882, -58.378330123 -34.5727671058, -58.3783302156 -34.5727671239, -58.378330282 -34.5727671365, -58.3783359446 -34.5727682501, -58.3783485141 -34.5727706386, -58.3783502411 -34.572770968, -58.3783572112 -34.5727722889, -58.3783779983 -34.5727731218, -58.3784087366 -34.5727757319, -58.3784549657 -34.5727802206, -58.3835240687 -34.5731844665, -58.3835298816 -34.573184573, -58.3835341448 -34.5731846488, -58.383535591 -34.573184675, -58.3835468158 -34.5731848715, -58.3835468474 -34.573184877, -58.3835469607 -34.5731848969, -58.383555134 -34.5731862544, -58.3835653308 -34.5731879476, -58.3835752917 -34.5731923991, -58.3835754791 -34.573192483, -58.3835755227 -34.5731925092, -58.3835757318 -34.5731926364, -58.3835762862 -34.5731929757, -58.3835839529 -34.5731976673, -58.3835862908 -34.5731996836, -58.3835901945 -34.5732030467, -58.3835958477 -34.5732095597, -58.3835978583 -34.5732130577, -58.3836001007 -34.5732169615, -58.3836015652 -34.573221806, -58.3836023974 -34.5732245595, -58.3836021272 -34.5732348593, -58.3836004084 -34.5732476533, -58.3835933033 -34.5733277675, -58.3835886337 -34.5733804612, -58.3835886293 -34.5733804955, -58.3835875063 -34.5733856041, -58.3835864162 -34.5733905253, -58.3835854639 -34.5733949715, -58.3835848465 -34.573397826, -58.3835848399 -34.5733978603, -58.3835848235 -34.5733979225, -58.3835835776 -34.5734039505, -58.38358357 -34.5734039884, -58.3835805951 -34.5734117182, -58.3835723389 -34.5734195878, -58.3835654294 -34.573424288, -58.3835621688 -34.5734265062, -58.3835527376 -34.573431165, -58.3835523723 -34.5734313451, -58.3835523254 -34.5734313685, -58.3835430287 -34.5734366963, -58.3825219845 -34.5740165823, -58.3821245883 -34.5742422727, -58.3818908423 -34.5743750211, -58.3818907397 -34.574375104, -58.3818906558 -34.5743751697, -58.3818806706 -34.5743832869, -58.3818806335 -34.5743833167, -58.3818679948 -34.5743890478, -58.3818606411 -34.5743931472, -58.3818605877 -34.5743931769, -58.3818603772 -34.574393294, -58.3818564474 -34.5743954846, -58.3818510378 -34.5743985577, -58.381844335 -34.5744023663, -58.3818417934 -34.5744035906, -58.3818397164 -34.5744045889, -58.3818356255 -34.5744065631, -58.3818294842 -34.5744078265, -58.3818222335 -34.574409072, -58.3818173103 -34.5744096258, -58.3818116611 -34.5744102585, -58.3817936882 -34.5744076459, -58.3817811079 -34.5744059194, -58.3817668593 -34.5744039619, -58.3801593912 -34.574275778, -58.3792746572 -34.5742052152, -58.3792587428 -34.5742039459, -58.3792438005 -34.5742027539, -58.3761133156 -34.5739530308, -58.3755141868 -34.5739056174, -58.3754384929 -34.5739252274, -58.3741073398 -34.5746894604, -58.3732950335 -34.5751558038, -58.3723292643 -34.5757054175, -58.3723105556 -34.5757160641, -58.3707608344 -34.576597975, -58.3707607974 -34.5765979966, -58.3707606469 -34.5765980776, -58.3707560014 -34.576600582, -58.3707493872 -34.5766054277, -58.3707481489 -34.5766065788, -58.3707453277 -34.5766092017, -58.3707423319 -34.5766149867, -58.3707422882 -34.5766150696, -58.3707422379 -34.5766152003, -58.3707414652 -34.5766171567, -58.3707414456 -34.5766172054, -58.3707397811 -34.5766214157, -58.3707392103 -34.576628049, -58.3706957935 -34.5770153181, -58.3706957935 -34.5770153568, -58.3706957934 -34.5770154271, -58.3706956893 -34.5770237952, -58.3706976097 -34.5770307332, -58.3706997962 -34.577037411, -58.370699807 -34.5770374417, -58.3707034703 -34.5770421085, -58.3707034954 -34.577042141, -58.370708723 -34.5770494034, -58.3707135885 -34.5770530489, -58.3707172572 -34.5770557974, -58.3707173247 -34.5770558489, -58.3707203706 -34.577057069, -58.3707266138 -34.5770595662, -58.3707359423 -34.5770621352, -58.3707442772 -34.5770623812, -58.3707528335 -34.577063555, -58.3707612606 -34.5770641627, -58.3707691789 -34.5770647338, -58.3760050692 -34.5774788735, -58.3760094074 -34.5774793544, -58.3760096853 -34.5774793852, -58.3760107119 -34.5774794977, -58.376016409 -34.5774801283, -58.3760409692 -34.5774840706, -58.3763758449 -34.5775146569, -58.3767109137 -34.5775452604, -58.3766902542 -34.5775570043, -58.3766902248 -34.5775570205, -58.3765861976 -34.5776161559, -58.373971723 -34.5791023036, -58.3751214877 -34.5805200713, -58.3761600512 -34.5799504792, -58.376933251 -34.5799949579, -58.3798362675 -34.5801619116, -58.3828568286 -34.5784486431, -58.3830652592 -34.578367367, -58.3832304075 -34.578314585, -58.3833992942 -34.5782705384, -58.3835712371 -34.5782352962, -58.3837454709 -34.5782091409, -58.3839213135 -34.5781919999, -58.3840981696 -34.5781840857, -58.3842752721 -34.5781853264, -58.3844506571 -34.5781957208, -58.3844518548 -34.5781957919, -58.3846274079 -34.5782153422, -58.3850633259 -34.5782472412, -58.3852863239 -34.5782463263, -58.3855087375 -34.5782338614, -58.3856189879 -34.578220486, -58.3857298832 -34.578209845, -58.3859493836 -34.5782173075, -58.3861234008 -34.5782113843, -58.3862957017 -34.5781849879, -58.3864087113 -34.5781623115, -58.3865198527 -34.578133788, -58.3865369064 -34.5781284161, -58.3865422755 -34.5781267247, -58.3865803577 -34.5781147313, -58.3868969975 -34.5781225916, -58.3875819304 -34.5781408456, -58.3882481717 -34.5781585976, -58.3883944668 -34.5781624954, -58.3894866704 -34.5781915888, -58.3896621145 -34.5781962616, -58.3898645519 -34.5782016524, -58.3898913402 -34.5782411256, -58.390387215 -34.5789717908, -58.3911944887 -34.5801614465, -58.3912155089 -34.5801927038, -58.3916441375 -34.5808302383, -58.3916446426 -34.5808309895, -58.3916347171 -34.5808333013, -58.3916264801 -34.5808352193, -58.3915322855 -34.5808592501, -58.3914575062 -34.5808807565, -58.3913929453 -34.5809029737, -58.3913393681 -34.5809242814, -58.3912973483 -34.580942996, -5</t>
-  </si>
-  <si>
-    <t>(-58.46681471374262, -34.590124613200004)</t>
-  </si>
-  <si>
-    <t>(-58.50082020879522, -34.6029645141)</t>
-  </si>
-  <si>
-    <t>(-58.420549629235715, -34.618844705149996)</t>
-  </si>
-  <si>
-    <t>(-58.443458670551706, -34.6168738474)</t>
-  </si>
-  <si>
-    <t>(-58.50312909088126, -34.627489216049995)</t>
-  </si>
-  <si>
-    <t>(-58.44834809731838, -34.63526070465)</t>
-  </si>
-  <si>
-    <t>(-58.37920119008943, -34.605895270000005)</t>
-  </si>
-  <si>
-    <t>(-58.40227541693436, -34.614390757500004)</t>
-  </si>
-  <si>
-    <t>(-58.39171430943253, -34.6399410959)</t>
-  </si>
-  <si>
-    <t>(-58.496753683151084, -34.653745497749995)</t>
-  </si>
-  <si>
-    <t>(-58.468149405695414, -34.678105831500005)</t>
-  </si>
-  <si>
-    <t>(-58.49057305775164, -34.5662573963)</t>
-  </si>
-  <si>
-    <t>(-58.4542381957974, -34.5547879506)</t>
-  </si>
-  <si>
-    <t>(-58.4227097595994, -34.5742740839)</t>
-  </si>
-  <si>
-    <t>(-58.393353948859556, -34.584020127849996)</t>
   </si>
 </sst>
 </file>
@@ -518,13 +425,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,263 +441,215 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>674.6383437985774</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>580.5230777036508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3">
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>553.7363659165568</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>481.2914316608345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>708.6426265992786</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>604.207040228952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5">
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>452.7135326292</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>394.7674525610054</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
+      <c r="B6">
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>582.803505817305</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>503.781597415267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="B7">
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>696.036500999695</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>597.5264848813511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>913.1572658954777</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>769.4314394248129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
+      <c r="B9">
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>923.282675629532</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>776.8439766635388</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="B10">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>1297.681220115204</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1117.418531063737</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
+      <c r="B11">
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>787.3745961450975</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>675.935351011776</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="B12">
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>859.3202073505843</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>743.0261290939844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
+      <c r="B13">
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>586.8741909488881</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>511.7916309443985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
+      <c r="B14">
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>361.1117439155642</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>311.6061104246527</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
+      <c r="B15">
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D15">
-        <v>464.0251400470056</v>
-      </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>392.8923969469731</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>238.6020806679211</v>
-      </c>
-      <c r="E16" t="s">
-        <v>48</v>
+        <v>201.9573471704984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>